<commit_message>
Test commit large files
</commit_message>
<xml_diff>
--- a/Dev Assets/ingredients.xlsx
+++ b/Dev Assets/ingredients.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="399">
   <si>
     <t xml:space="preserve">Ingredients</t>
   </si>
@@ -175,7 +175,7 @@
     <t xml:space="preserve">tongues</t>
   </si>
   <si>
-    <t xml:space="preserve">bundle</t>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">DECAY</t>
@@ -793,7 +793,7 @@
     <t xml:space="preserve">ff</t>
   </si>
   <si>
-    <t xml:space="preserve">aa</t>
+    <t xml:space="preserve">ambergris</t>
   </si>
   <si>
     <t xml:space="preserve">fg</t>
@@ -1540,6 +1540,112 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -1547,14 +1653,14 @@
   </sheetPr>
   <dimension ref="A1:S224"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B14" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E102" activeCellId="0" sqref="E102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="36.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="29.71"/>
@@ -1894,7 +2000,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I14" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E15" s="5" t="s">
         <v>73</v>

</xml_diff>